<commit_message>
Test Design updated for UserService
</commit_message>
<xml_diff>
--- a/TestDesign/CheckList_user.xlsx
+++ b/TestDesign/CheckList_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Escritorio\AQA Bootcamp\Tasks\HTTP-Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Escritorio\AQA Bootcamp\Tasks\HTTP-Task\UserService-WalletService_BackendAutoTests\TestDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A4F0E7-9772-4318-8D0C-F38CDDFF09D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9B6D1C-76DF-4B14-9EC3-26AB267060C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2865" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserServiceTestIdeas" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>N</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Method Tested</t>
   </si>
   <si>
-    <t>Register User With Empty fields</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -133,6 +130,38 @@
   </si>
   <si>
     <t>Response Body is: ID &gt; 0</t>
+  </si>
+  <si>
+    <t>Fields With Special Characters</t>
+  </si>
+  <si>
+    <t>Fields Are Upper Case</t>
+  </si>
+  <si>
+    <t>With Empty fields</t>
+  </si>
+  <si>
+    <t>Fields Length = 1 Symbol</t>
+  </si>
+  <si>
+    <t>Fields Length &gt; 100 Symbols</t>
+  </si>
+  <si>
+    <t>Register two Users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response Value (ID) is autoincremented. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response Code Is 200
+ID should be n+1. </t>
+  </si>
+  <si>
+    <t>Fields = Null</t>
+  </si>
+  <si>
+    <t>Response Code Is 200
+Body is ID &gt; 0</t>
   </si>
 </sst>
 </file>
@@ -193,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -216,11 +245,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +269,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,22 +617,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -604,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -615,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -626,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -637,7 +687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -647,8 +697,9 @@
       <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -659,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -670,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -681,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -692,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -714,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -725,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -736,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -859,29 +910,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -892,19 +945,22 @@
         <v>25</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -912,20 +968,23 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -933,97 +992,157 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="6"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1033,8 +1152,9 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1044,8 +1164,9 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1055,8 +1176,9 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1066,8 +1188,9 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1077,8 +1200,9 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1086,8 +1210,9 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1095,8 +1220,9 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1104,8 +1230,9 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1113,8 +1240,9 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1122,8 +1250,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1131,8 +1260,9 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1140,8 +1270,9 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1149,8 +1280,9 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1158,8 +1290,9 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1167,8 +1300,9 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1176,9 +1310,10 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="7"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3 more User Service Register User tests added.
</commit_message>
<xml_diff>
--- a/TestDesign/CheckList_user.xlsx
+++ b/TestDesign/CheckList_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Escritorio\AQA Bootcamp\Tasks\HTTP-Task\UserService-WalletService_BackendAutoTests\TestDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D655559-774D-46A0-AFB2-91A92332D0A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C63BDBD-198C-4E28-9E22-5FFE974B8CD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="2865" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
   <si>
     <t>N</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Response Code Is 200</t>
-  </si>
-  <si>
-    <t>Response Body is: ID &gt; 0</t>
   </si>
   <si>
     <t>Fields With Special Characters</t>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Fields are digits</t>
+  </si>
+  <si>
+    <t>Response Code Is 500</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -957,13 +957,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
+      <c r="E2" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>32</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -981,13 +981,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>35</v>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>32</v>
@@ -1005,16 +1005,20 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="6">
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1027,15 +1031,20 @@
       <c r="C5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="10">
         <v>3</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="6"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1047,75 +1056,91 @@
       <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="10">
-        <v>3</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="C7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="10">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="10">
-        <v>3</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1125,35 +1150,33 @@
       <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>11</v>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>45</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1162,12 +1185,6 @@
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>

</xml_diff>